<commit_message>
added fall2022 program files
</commit_message>
<xml_diff>
--- a/Fall2022_program/round_1_match.xlsx
+++ b/Fall2022_program/round_1_match.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/saunders/Documents/BU_grad_trios/Fall2022_program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DC2D97BC-55CE-154F-B198-2F1F0A5B4652}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47972C76-C5CC-124E-999A-E8CF1C3673B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="1500" windowWidth="27640" windowHeight="16940"/>
+    <workbookView xWindow="5120" yWindow="1500" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="round_1_match" sheetId="1" r:id="rId1"/>
@@ -1810,9 +1810,6 @@
     <t>Jae Hyung Sim</t>
   </si>
   <si>
-    <t>simjhsim</t>
-  </si>
-  <si>
     <t>Francesca Camacho</t>
   </si>
   <si>
@@ -2090,13 +2087,16 @@
   </si>
   <si>
     <t>wsaund@bu.edu</t>
+  </si>
+  <si>
+    <t>simjhsim@bu.edu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2227,6 +2227,14 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2529,7 +2537,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2572,12 +2580,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2611,6 +2621,7 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -2930,14 +2941,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H218"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A167" workbookViewId="0">
+      <selection activeCell="D188" sqref="D188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="31.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -7539,8 +7553,8 @@
       <c r="C187">
         <v>44883229</v>
       </c>
-      <c r="D187" t="s">
-        <v>596</v>
+      <c r="D187" s="2" t="s">
+        <v>689</v>
       </c>
       <c r="E187" t="s">
         <v>16</v>
@@ -7554,16 +7568,16 @@
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
+        <v>596</v>
+      </c>
+      <c r="B188" t="s">
         <v>597</v>
-      </c>
-      <c r="B188" t="s">
-        <v>598</v>
       </c>
       <c r="C188">
         <v>57193951</v>
       </c>
       <c r="D188" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="E188" t="s">
         <v>43</v>
@@ -7577,16 +7591,16 @@
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
+        <v>599</v>
+      </c>
+      <c r="B189" t="s">
         <v>600</v>
-      </c>
-      <c r="B189" t="s">
-        <v>601</v>
       </c>
       <c r="C189">
         <v>60749518</v>
       </c>
       <c r="D189" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="E189" t="s">
         <v>43</v>
@@ -7603,22 +7617,22 @@
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
+        <v>602</v>
+      </c>
+      <c r="B190" t="s">
         <v>603</v>
-      </c>
-      <c r="B190" t="s">
-        <v>604</v>
       </c>
       <c r="C190">
         <v>30673885</v>
       </c>
       <c r="D190" t="s">
+        <v>604</v>
+      </c>
+      <c r="E190" t="s">
+        <v>16</v>
+      </c>
+      <c r="F190" t="s">
         <v>605</v>
-      </c>
-      <c r="E190" t="s">
-        <v>16</v>
-      </c>
-      <c r="F190" t="s">
-        <v>606</v>
       </c>
       <c r="G190" t="s">
         <v>12</v>
@@ -7626,16 +7640,16 @@
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
+        <v>606</v>
+      </c>
+      <c r="B191" t="s">
         <v>607</v>
-      </c>
-      <c r="B191" t="s">
-        <v>608</v>
       </c>
       <c r="C191">
         <v>98345155</v>
       </c>
       <c r="D191" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="E191" t="s">
         <v>21</v>
@@ -7652,16 +7666,16 @@
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
+        <v>609</v>
+      </c>
+      <c r="B192" t="s">
         <v>610</v>
-      </c>
-      <c r="B192" t="s">
-        <v>611</v>
       </c>
       <c r="C192">
         <v>7046454</v>
       </c>
       <c r="D192" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E192" t="s">
         <v>43</v>
@@ -7678,16 +7692,16 @@
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
+        <v>612</v>
+      </c>
+      <c r="B193" t="s">
         <v>613</v>
-      </c>
-      <c r="B193" t="s">
-        <v>614</v>
       </c>
       <c r="C193">
         <v>1305380</v>
       </c>
       <c r="D193" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="E193" t="s">
         <v>43</v>
@@ -7704,16 +7718,16 @@
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
+        <v>615</v>
+      </c>
+      <c r="B194" t="s">
         <v>616</v>
-      </c>
-      <c r="B194" t="s">
-        <v>617</v>
       </c>
       <c r="C194">
         <v>72418396</v>
       </c>
       <c r="D194" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E194" t="s">
         <v>43</v>
@@ -7730,16 +7744,16 @@
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
+        <v>618</v>
+      </c>
+      <c r="B195" t="s">
         <v>619</v>
-      </c>
-      <c r="B195" t="s">
-        <v>620</v>
       </c>
       <c r="C195">
         <v>61160628</v>
       </c>
       <c r="D195" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="E195" t="s">
         <v>16</v>
@@ -7756,16 +7770,16 @@
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
+        <v>621</v>
+      </c>
+      <c r="B196" t="s">
         <v>622</v>
-      </c>
-      <c r="B196" t="s">
-        <v>623</v>
       </c>
       <c r="C196">
         <v>38366338</v>
       </c>
       <c r="D196" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="E196" t="s">
         <v>16</v>
@@ -7779,16 +7793,16 @@
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
+        <v>624</v>
+      </c>
+      <c r="B197" t="s">
         <v>625</v>
-      </c>
-      <c r="B197" t="s">
-        <v>626</v>
       </c>
       <c r="C197">
         <v>25978414</v>
       </c>
       <c r="D197" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
       <c r="E197" t="s">
         <v>43</v>
@@ -7802,16 +7816,16 @@
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
+        <v>627</v>
+      </c>
+      <c r="B198" t="s">
         <v>628</v>
-      </c>
-      <c r="B198" t="s">
-        <v>629</v>
       </c>
       <c r="C198">
         <v>77222659</v>
       </c>
       <c r="D198" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
       <c r="E198" t="s">
         <v>16</v>
@@ -7828,7 +7842,7 @@
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
       <c r="B199" t="s">
         <v>159</v>
@@ -7837,7 +7851,7 @@
         <v>38057241</v>
       </c>
       <c r="D199" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
       <c r="E199" t="s">
         <v>16</v>
@@ -7851,16 +7865,16 @@
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
+        <v>632</v>
+      </c>
+      <c r="B200" t="s">
         <v>633</v>
-      </c>
-      <c r="B200" t="s">
-        <v>634</v>
       </c>
       <c r="C200">
         <v>73848659</v>
       </c>
       <c r="D200" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
       <c r="E200" t="s">
         <v>43</v>
@@ -7877,16 +7891,16 @@
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
+        <v>635</v>
+      </c>
+      <c r="B201" t="s">
         <v>636</v>
-      </c>
-      <c r="B201" t="s">
-        <v>637</v>
       </c>
       <c r="C201">
         <v>76804636</v>
       </c>
       <c r="D201" t="s">
-        <v>638</v>
+        <v>637</v>
       </c>
       <c r="E201" t="s">
         <v>16</v>
@@ -7903,16 +7917,16 @@
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
+        <v>638</v>
+      </c>
+      <c r="B202" t="s">
         <v>639</v>
-      </c>
-      <c r="B202" t="s">
-        <v>640</v>
       </c>
       <c r="C202">
         <v>43766257</v>
       </c>
       <c r="D202" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
       <c r="E202" t="s">
         <v>21</v>
@@ -7926,16 +7940,16 @@
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
+        <v>641</v>
+      </c>
+      <c r="B203" t="s">
         <v>642</v>
-      </c>
-      <c r="B203" t="s">
-        <v>643</v>
       </c>
       <c r="C203">
         <v>25314384</v>
       </c>
       <c r="D203" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
       <c r="E203" t="s">
         <v>43</v>
@@ -7952,16 +7966,16 @@
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
+        <v>644</v>
+      </c>
+      <c r="B204" t="s">
         <v>645</v>
-      </c>
-      <c r="B204" t="s">
-        <v>646</v>
       </c>
       <c r="C204">
         <v>297553354</v>
       </c>
       <c r="D204" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
       <c r="E204" t="s">
         <v>79</v>
@@ -7975,16 +7989,16 @@
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
+        <v>647</v>
+      </c>
+      <c r="B205" t="s">
         <v>648</v>
-      </c>
-      <c r="B205" t="s">
-        <v>649</v>
       </c>
       <c r="C205">
         <v>18356467</v>
       </c>
       <c r="D205" t="s">
-        <v>650</v>
+        <v>649</v>
       </c>
       <c r="E205" t="s">
         <v>21</v>
@@ -8001,16 +8015,16 @@
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
+        <v>650</v>
+      </c>
+      <c r="B206" t="s">
         <v>651</v>
-      </c>
-      <c r="B206" t="s">
-        <v>652</v>
       </c>
       <c r="C206">
         <v>29168211</v>
       </c>
       <c r="D206" t="s">
-        <v>653</v>
+        <v>652</v>
       </c>
       <c r="E206" t="s">
         <v>21</v>
@@ -8024,16 +8038,16 @@
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
+        <v>653</v>
+      </c>
+      <c r="B207" t="s">
         <v>654</v>
-      </c>
-      <c r="B207" t="s">
-        <v>655</v>
       </c>
       <c r="C207">
         <v>35740812</v>
       </c>
       <c r="D207" t="s">
-        <v>656</v>
+        <v>655</v>
       </c>
       <c r="E207" t="s">
         <v>43</v>
@@ -8050,16 +8064,16 @@
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>656</v>
+      </c>
+      <c r="B208" t="s">
         <v>657</v>
-      </c>
-      <c r="B208" t="s">
-        <v>658</v>
       </c>
       <c r="C208">
         <v>32581362</v>
       </c>
       <c r="D208" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="E208" t="s">
         <v>16</v>
@@ -8076,16 +8090,16 @@
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
+        <v>659</v>
+      </c>
+      <c r="B209" t="s">
         <v>660</v>
-      </c>
-      <c r="B209" t="s">
-        <v>661</v>
       </c>
       <c r="C209">
         <v>6886967</v>
       </c>
       <c r="D209" t="s">
-        <v>662</v>
+        <v>661</v>
       </c>
       <c r="E209" t="s">
         <v>16</v>
@@ -8102,16 +8116,16 @@
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
+        <v>662</v>
+      </c>
+      <c r="B210" t="s">
         <v>663</v>
-      </c>
-      <c r="B210" t="s">
-        <v>664</v>
       </c>
       <c r="C210">
         <v>76233090</v>
       </c>
       <c r="D210" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E210" t="s">
         <v>16</v>
@@ -8128,16 +8142,16 @@
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
+        <v>665</v>
+      </c>
+      <c r="B211" t="s">
         <v>666</v>
-      </c>
-      <c r="B211" t="s">
-        <v>667</v>
       </c>
       <c r="C211">
         <v>55006554</v>
       </c>
       <c r="D211" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E211" t="s">
         <v>89</v>
@@ -8154,16 +8168,16 @@
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
+        <v>668</v>
+      </c>
+      <c r="B212" t="s">
         <v>669</v>
-      </c>
-      <c r="B212" t="s">
-        <v>670</v>
       </c>
       <c r="C212">
         <v>63437935</v>
       </c>
       <c r="D212" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E212" t="s">
         <v>79</v>
@@ -8180,16 +8194,16 @@
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
+        <v>671</v>
+      </c>
+      <c r="B213" t="s">
         <v>672</v>
-      </c>
-      <c r="B213" t="s">
-        <v>673</v>
       </c>
       <c r="C213">
         <v>27136704</v>
       </c>
       <c r="D213" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E213" t="s">
         <v>79</v>
@@ -8206,16 +8220,16 @@
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
+        <v>674</v>
+      </c>
+      <c r="B214" t="s">
         <v>675</v>
-      </c>
-      <c r="B214" t="s">
-        <v>676</v>
       </c>
       <c r="C214">
         <v>14202533</v>
       </c>
       <c r="D214" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E214" t="s">
         <v>16</v>
@@ -8232,16 +8246,16 @@
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
+        <v>677</v>
+      </c>
+      <c r="B215" t="s">
         <v>678</v>
-      </c>
-      <c r="B215" t="s">
-        <v>679</v>
       </c>
       <c r="C215">
         <v>10515972</v>
       </c>
       <c r="D215" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E215" t="s">
         <v>386</v>
@@ -8255,16 +8269,16 @@
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
+        <v>680</v>
+      </c>
+      <c r="B216" t="s">
         <v>681</v>
-      </c>
-      <c r="B216" t="s">
-        <v>682</v>
       </c>
       <c r="C216">
         <v>80884705</v>
       </c>
       <c r="D216" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E216" t="s">
         <v>16</v>
@@ -8278,16 +8292,16 @@
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
+        <v>683</v>
+      </c>
+      <c r="B217" t="s">
         <v>684</v>
-      </c>
-      <c r="B217" t="s">
-        <v>685</v>
       </c>
       <c r="C217">
         <v>27652521</v>
       </c>
       <c r="D217" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E217" t="s">
         <v>16</v>
@@ -8304,16 +8318,16 @@
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
+        <v>686</v>
+      </c>
+      <c r="B218" t="s">
         <v>687</v>
-      </c>
-      <c r="B218" t="s">
-        <v>688</v>
       </c>
       <c r="C218">
         <v>90747427</v>
       </c>
       <c r="D218" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E218" t="s">
         <v>16</v>
@@ -8329,6 +8343,9 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D187" r:id="rId1" xr:uid="{13CD0774-6775-4043-8429-EDE1E0606DFA}"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>